<commit_message>
Actualizacion lista de precios mar 16/09/2025 21:18:36,62
</commit_message>
<xml_diff>
--- a/upload/lista.xlsx
+++ b/upload/lista.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Empresa 1</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>1001.88</t>
+  </si>
+  <si>
+    <t>Empresa 3</t>
+  </si>
+  <si>
+    <t>Papitas</t>
   </si>
 </sst>
 </file>
@@ -376,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,6 +469,17 @@
       </c>
       <c r="C7">
         <v>34343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion lista de precios mar 16/09/2025 21:21:04,15
</commit_message>
<xml_diff>
--- a/upload/lista.xlsx
+++ b/upload/lista.xlsx
@@ -385,7 +385,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +479,7 @@
         <v>14</v>
       </c>
       <c r="C8">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion lista de precios mar 16/09/2025 21:23:58,49
</commit_message>
<xml_diff>
--- a/upload/lista.xlsx
+++ b/upload/lista.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Empresa 1</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Articulo agregado</t>
-  </si>
-  <si>
-    <t>1001.88</t>
   </si>
   <si>
     <t>Empresa 3</t>
@@ -385,7 +382,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,8 +398,8 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
+      <c r="C1">
+        <v>1002</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -473,10 +470,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
       </c>
       <c r="C8">
         <v>201</v>

</xml_diff>

<commit_message>
Actualizacion lista de precios mar 16/09/2025 21:27:55,59
</commit_message>
<xml_diff>
--- a/upload/lista.xlsx
+++ b/upload/lista.xlsx
@@ -382,7 +382,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion lista de precios mar 16/09/2025 21:54:51,48
</commit_message>
<xml_diff>
--- a/upload/lista.xlsx
+++ b/upload/lista.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Empresa 1</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>Papitas</t>
+  </si>
+  <si>
+    <t>Empresa 4</t>
+  </si>
+  <si>
+    <t>Azúcar x1kg</t>
+  </si>
+  <si>
+    <t>Sal x1kg</t>
   </si>
 </sst>
 </file>
@@ -379,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,6 +486,28 @@
       </c>
       <c r="C8">
         <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion lista de precios mar 16/09/2025 22:00:10,59
</commit_message>
<xml_diff>
--- a/upload/lista.xlsx
+++ b/upload/lista.xlsx
@@ -67,16 +67,19 @@
     <t>Empresa 4</t>
   </si>
   <si>
-    <t>Azúcar x1kg</t>
-  </si>
-  <si>
     <t>Sal x1kg</t>
+  </si>
+  <si>
+    <t>Azucar x1kg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;\ #,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,8 +109,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,13 +395,14 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -407,8 +412,8 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>1002</v>
+      <c r="C1" s="1">
+        <v>1003</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -418,8 +423,8 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>12121</v>
+      <c r="C2" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -429,8 +434,8 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>122121</v>
+      <c r="C3" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -440,7 +445,7 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -451,7 +456,7 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -462,7 +467,7 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -473,7 +478,7 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>34343</v>
       </c>
     </row>
@@ -484,7 +489,7 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>202</v>
       </c>
     </row>
@@ -493,9 +498,9 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1">
         <v>800</v>
       </c>
     </row>
@@ -504,9 +509,9 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1">
         <v>900</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizacion lista de precios mar 16/09/2025 22:01:28,76
</commit_message>
<xml_diff>
--- a/upload/lista.xlsx
+++ b/upload/lista.xlsx
@@ -78,7 +78,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -111,7 +111,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +395,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +424,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualizacion lista de precios lun 22/09/2025  9:40:33,37
</commit_message>
<xml_diff>
--- a/upload/lista.xlsx
+++ b/upload/lista.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lista" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Empresa 1</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Azucar x1kg</t>
+  </si>
+  <si>
+    <t>Articulo 78</t>
+  </si>
+  <si>
+    <t>Articulo 9</t>
   </si>
 </sst>
 </file>
@@ -394,7 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -522,12 +528,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>5490</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion lista de precios lun 22/09/2025 15:05:28,49
</commit_message>
<xml_diff>
--- a/upload/lista.xlsx
+++ b/upload/lista.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Empresa 1</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Articulo 9</t>
+  </si>
+  <si>
+    <t>Articulo 57</t>
   </si>
 </sst>
 </file>
@@ -528,10 +531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,6 +583,17 @@
         <v>1200</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>2000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizacion lista de precios lun 22/09/2025 20:32:01,55
</commit_message>
<xml_diff>
--- a/upload/lista.xlsx
+++ b/upload/lista.xlsx
@@ -534,7 +534,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +547,7 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>2200</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualizacion lista de precios lun 22/09/2025 20:33:29,66
</commit_message>
<xml_diff>
--- a/upload/lista.xlsx
+++ b/upload/lista.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Lista" sheetId="1" r:id="rId1"/>
@@ -403,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +422,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1">
-        <v>1003</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -533,7 +533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>